<commit_message>
Added default route for green line in Line Class
</commit_message>
<xml_diff>
--- a/CTC_App/Iteration3/Track_Layout_Green.xlsx
+++ b/CTC_App/Iteration3/Track_Layout_Green.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="181" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="180" uniqueCount="55">
   <si>
     <t xml:space="preserve">Line</t>
   </si>
@@ -160,16 +160,16 @@
     <t xml:space="preserve">U</t>
   </si>
   <si>
+    <t xml:space="preserve">GLENBURY U</t>
+  </si>
+  <si>
+    <t xml:space="preserve">V</t>
+  </si>
+  <si>
+    <t xml:space="preserve">W</t>
+  </si>
+  <si>
     <t xml:space="preserve">OVERBROOK W</t>
-  </si>
-  <si>
-    <t xml:space="preserve">GLENBURY U</t>
-  </si>
-  <si>
-    <t xml:space="preserve">V</t>
-  </si>
-  <si>
-    <t xml:space="preserve">W</t>
   </si>
   <si>
     <t xml:space="preserve">INGLEWOOD W</t>
@@ -331,12 +331,12 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:K152"/>
+  <dimension ref="A1:I152"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="78" zoomScaleNormal="78" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <pane xSplit="0" ySplit="1" topLeftCell="A86" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="H21" activeCellId="0" sqref="H21"/>
+      <selection pane="bottomLeft" activeCell="K110" activeCellId="0" sqref="K110:K119"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.80859375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -3799,9 +3799,6 @@
       <c r="I115" s="2" t="n">
         <v>-1</v>
       </c>
-      <c r="K115" s="2" t="s">
-        <v>46</v>
-      </c>
     </row>
     <row r="116" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A116" s="1" t="str">
@@ -3828,7 +3825,7 @@
         <v>-1</v>
       </c>
       <c r="H116" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="I116" s="2" t="n">
         <v>-1</v>
@@ -3900,7 +3897,7 @@
         <v>Green</v>
       </c>
       <c r="B119" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C119" s="1" t="n">
         <v>117</v>
@@ -3930,7 +3927,7 @@
         <v>Green</v>
       </c>
       <c r="B120" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C120" s="7" t="n">
         <v>118</v>
@@ -3960,7 +3957,7 @@
         <v>Green</v>
       </c>
       <c r="B121" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C121" s="1" t="n">
         <v>119</v>
@@ -3990,7 +3987,7 @@
         <v>Green</v>
       </c>
       <c r="B122" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C122" s="1" t="n">
         <v>120</v>
@@ -4020,7 +4017,7 @@
         <v>Green</v>
       </c>
       <c r="B123" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C123" s="1" t="n">
         <v>121</v>
@@ -4050,7 +4047,7 @@
         <v>Green</v>
       </c>
       <c r="B124" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C124" s="7" t="n">
         <v>122</v>
@@ -4080,7 +4077,7 @@
         <v>Green</v>
       </c>
       <c r="B125" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C125" s="1" t="n">
         <v>123</v>
@@ -4098,7 +4095,7 @@
         <v>-1</v>
       </c>
       <c r="H125" s="1" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
       <c r="I125" s="2" t="n">
         <v>-1</v>
@@ -4110,7 +4107,7 @@
         <v>Green</v>
       </c>
       <c r="B126" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C126" s="1" t="n">
         <v>124</v>
@@ -4140,7 +4137,7 @@
         <v>Green</v>
       </c>
       <c r="B127" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C127" s="1" t="n">
         <v>125</v>
@@ -4170,7 +4167,7 @@
         <v>Green</v>
       </c>
       <c r="B128" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C128" s="7" t="n">
         <v>126</v>
@@ -4200,7 +4197,7 @@
         <v>Green</v>
       </c>
       <c r="B129" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C129" s="1" t="n">
         <v>127</v>
@@ -4230,7 +4227,7 @@
         <v>Green</v>
       </c>
       <c r="B130" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C130" s="1" t="n">
         <v>128</v>
@@ -4260,7 +4257,7 @@
         <v>Green</v>
       </c>
       <c r="B131" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C131" s="1" t="n">
         <v>129</v>
@@ -4290,7 +4287,7 @@
         <v>Green</v>
       </c>
       <c r="B132" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C132" s="7" t="n">
         <v>130</v>
@@ -4320,7 +4317,7 @@
         <v>Green</v>
       </c>
       <c r="B133" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C133" s="1" t="n">
         <v>131</v>
@@ -4350,7 +4347,7 @@
         <v>Green</v>
       </c>
       <c r="B134" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C134" s="1" t="n">
         <v>132</v>
@@ -4380,7 +4377,7 @@
         <v>Green</v>
       </c>
       <c r="B135" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C135" s="1" t="n">
         <v>133</v>
@@ -4410,7 +4407,7 @@
         <v>Green</v>
       </c>
       <c r="B136" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C136" s="7" t="n">
         <v>134</v>
@@ -4440,7 +4437,7 @@
         <v>Green</v>
       </c>
       <c r="B137" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C137" s="1" t="n">
         <v>135</v>
@@ -4470,7 +4467,7 @@
         <v>Green</v>
       </c>
       <c r="B138" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C138" s="1" t="n">
         <v>136</v>
@@ -4500,7 +4497,7 @@
         <v>Green</v>
       </c>
       <c r="B139" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C139" s="1" t="n">
         <v>137</v>
@@ -4530,7 +4527,7 @@
         <v>Green</v>
       </c>
       <c r="B140" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C140" s="7" t="n">
         <v>138</v>
@@ -4560,7 +4557,7 @@
         <v>Green</v>
       </c>
       <c r="B141" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C141" s="1" t="n">
         <v>139</v>
@@ -4590,7 +4587,7 @@
         <v>Green</v>
       </c>
       <c r="B142" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C142" s="1" t="n">
         <v>140</v>
@@ -4620,7 +4617,7 @@
         <v>Green</v>
       </c>
       <c r="B143" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C143" s="1" t="n">
         <v>141</v>
@@ -4650,7 +4647,7 @@
         <v>Green</v>
       </c>
       <c r="B144" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C144" s="7" t="n">
         <v>142</v>
@@ -4680,7 +4677,7 @@
         <v>Green</v>
       </c>
       <c r="B145" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C145" s="1" t="n">
         <v>143</v>

</xml_diff>

<commit_message>
Dispatch to specific blocks implemented and edit station implementation improved
</commit_message>
<xml_diff>
--- a/CTC_App/Iteration3/Track_Layout_Green.xlsx
+++ b/CTC_App/Iteration3/Track_Layout_Green.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\yasse\Desktop\ECE1140\Team_X_ECE_1140\CTC_App\Iteration3\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E952FF3F-C0BB-4946-BC8F-9755B0C6EC59}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BA58B05B-CE60-4375-9F2E-981A77A34F56}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3120" yWindow="3120" windowWidth="21600" windowHeight="11325" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Green Line" sheetId="1" r:id="rId1"/>
@@ -251,7 +251,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -263,7 +263,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="3" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="3" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="1" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
@@ -272,10 +272,6 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -594,7 +590,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="78" zoomScaleNormal="78" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="L19" sqref="L19"/>
+      <selection pane="bottomLeft" activeCell="K23" sqref="K23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -606,7 +602,7 @@
     <col min="5" max="5" width="13.28515625" style="1" customWidth="1"/>
     <col min="6" max="7" width="9.140625" style="1" customWidth="1"/>
     <col min="8" max="8" width="31" style="1" customWidth="1"/>
-    <col min="9" max="9" width="17.7109375" style="9" customWidth="1"/>
+    <col min="9" max="9" width="17.7109375" style="2" customWidth="1"/>
     <col min="10" max="10" width="11.42578125" style="2" customWidth="1"/>
     <col min="11" max="1020" width="8.7109375" style="2"/>
   </cols>
@@ -636,7 +632,7 @@
       <c r="H1" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="8" t="s">
+      <c r="I1" s="3" t="s">
         <v>8</v>
       </c>
     </row>
@@ -665,7 +661,7 @@
       <c r="H2" s="1">
         <v>-1</v>
       </c>
-      <c r="I2" s="9">
+      <c r="I2" s="2">
         <v>-1</v>
       </c>
     </row>
@@ -691,10 +687,10 @@
       <c r="G3" s="1">
         <v>-1</v>
       </c>
-      <c r="H3" s="1">
-        <v>-1</v>
-      </c>
-      <c r="I3" s="9">
+      <c r="H3" s="6">
+        <v>1</v>
+      </c>
+      <c r="I3" s="2">
         <v>-1</v>
       </c>
     </row>
@@ -724,7 +720,7 @@
       <c r="H4" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="I4" s="9">
+      <c r="I4" s="2">
         <v>-1</v>
       </c>
     </row>
@@ -752,9 +748,9 @@
         <v>-1</v>
       </c>
       <c r="H5" s="1">
-        <v>-1</v>
-      </c>
-      <c r="I5" s="9">
+        <v>3</v>
+      </c>
+      <c r="I5" s="2">
         <v>-1</v>
       </c>
     </row>
@@ -781,10 +777,10 @@
       <c r="G6" s="1">
         <v>-1</v>
       </c>
-      <c r="H6" s="1">
-        <v>-1</v>
-      </c>
-      <c r="I6" s="9">
+      <c r="H6" s="6">
+        <v>4</v>
+      </c>
+      <c r="I6" s="2">
         <v>-1</v>
       </c>
     </row>
@@ -812,9 +808,9 @@
         <v>-1</v>
       </c>
       <c r="H7" s="1">
-        <v>-1</v>
-      </c>
-      <c r="I7" s="9">
+        <v>5</v>
+      </c>
+      <c r="I7" s="2">
         <v>-1</v>
       </c>
     </row>
@@ -842,9 +838,9 @@
         <v>-1</v>
       </c>
       <c r="H8" s="1">
-        <v>-1</v>
-      </c>
-      <c r="I8" s="9">
+        <v>6</v>
+      </c>
+      <c r="I8" s="2">
         <v>-1</v>
       </c>
     </row>
@@ -871,10 +867,10 @@
       <c r="G9" s="1">
         <v>-1</v>
       </c>
-      <c r="H9" s="1">
-        <v>-1</v>
-      </c>
-      <c r="I9" s="9">
+      <c r="H9" s="6">
+        <v>7</v>
+      </c>
+      <c r="I9" s="2">
         <v>-1</v>
       </c>
     </row>
@@ -902,9 +898,9 @@
         <v>-1</v>
       </c>
       <c r="H10" s="1">
-        <v>-1</v>
-      </c>
-      <c r="I10" s="9">
+        <v>8</v>
+      </c>
+      <c r="I10" s="2">
         <v>-1</v>
       </c>
     </row>
@@ -934,7 +930,7 @@
       <c r="H11" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="I11" s="9">
+      <c r="I11" s="2">
         <v>-1</v>
       </c>
     </row>
@@ -961,10 +957,10 @@
       <c r="G12" s="1">
         <v>-1</v>
       </c>
-      <c r="H12" s="1">
-        <v>-1</v>
-      </c>
-      <c r="I12" s="9">
+      <c r="H12" s="6">
+        <v>10</v>
+      </c>
+      <c r="I12" s="2">
         <v>-1</v>
       </c>
     </row>
@@ -992,9 +988,9 @@
         <v>-1</v>
       </c>
       <c r="H13" s="1">
-        <v>-1</v>
-      </c>
-      <c r="I13" s="9">
+        <v>11</v>
+      </c>
+      <c r="I13" s="2">
         <v>-1</v>
       </c>
     </row>
@@ -1021,10 +1017,10 @@
       <c r="G14" s="1">
         <v>-1</v>
       </c>
-      <c r="H14" s="1">
-        <v>-1</v>
-      </c>
-      <c r="I14" s="9">
+      <c r="H14" s="6">
+        <v>12</v>
+      </c>
+      <c r="I14" s="2">
         <v>-1</v>
       </c>
     </row>
@@ -1052,9 +1048,9 @@
         <v>1</v>
       </c>
       <c r="H15" s="1">
-        <v>-1</v>
-      </c>
-      <c r="I15" s="9">
+        <v>13</v>
+      </c>
+      <c r="I15" s="2">
         <v>-1</v>
       </c>
     </row>
@@ -1082,9 +1078,9 @@
         <v>-1</v>
       </c>
       <c r="H16" s="1">
-        <v>-1</v>
-      </c>
-      <c r="I16" s="9">
+        <v>14</v>
+      </c>
+      <c r="I16" s="2">
         <v>-1</v>
       </c>
     </row>
@@ -1111,10 +1107,10 @@
       <c r="G17" s="1">
         <v>-1</v>
       </c>
-      <c r="H17" s="1">
-        <v>-1</v>
-      </c>
-      <c r="I17" s="9">
+      <c r="H17" s="6">
+        <v>15</v>
+      </c>
+      <c r="I17" s="2">
         <v>-1</v>
       </c>
     </row>
@@ -1144,7 +1140,7 @@
       <c r="H18" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="I18" s="9">
+      <c r="I18" s="2">
         <v>-1</v>
       </c>
     </row>
@@ -1171,10 +1167,10 @@
       <c r="G19" s="1">
         <v>-1</v>
       </c>
-      <c r="H19" s="1">
-        <v>-1</v>
-      </c>
-      <c r="I19" s="9">
+      <c r="H19" s="6">
+        <v>17</v>
+      </c>
+      <c r="I19" s="2">
         <v>-1</v>
       </c>
     </row>
@@ -1202,9 +1198,9 @@
         <v>-1</v>
       </c>
       <c r="H20" s="1">
-        <v>-1</v>
-      </c>
-      <c r="I20" s="9">
+        <v>18</v>
+      </c>
+      <c r="I20" s="2">
         <v>-1</v>
       </c>
     </row>
@@ -1231,10 +1227,10 @@
       <c r="G21" s="1">
         <v>-1</v>
       </c>
-      <c r="H21" s="7">
-        <v>-1</v>
-      </c>
-      <c r="I21" s="9">
+      <c r="H21" s="1">
+        <v>19</v>
+      </c>
+      <c r="I21" s="2">
         <v>1</v>
       </c>
     </row>
@@ -1261,10 +1257,10 @@
       <c r="G22" s="1">
         <v>-1</v>
       </c>
-      <c r="H22" s="1">
-        <v>-1</v>
-      </c>
-      <c r="I22" s="9">
+      <c r="H22" s="6">
+        <v>20</v>
+      </c>
+      <c r="I22" s="2">
         <v>-1</v>
       </c>
     </row>
@@ -1292,9 +1288,9 @@
         <v>-1</v>
       </c>
       <c r="H23" s="1">
-        <v>-1</v>
-      </c>
-      <c r="I23" s="9">
+        <v>21</v>
+      </c>
+      <c r="I23" s="2">
         <v>-1</v>
       </c>
     </row>
@@ -1324,7 +1320,7 @@
       <c r="H24" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="I24" s="9">
+      <c r="I24" s="2">
         <v>-1</v>
       </c>
     </row>
@@ -1352,9 +1348,9 @@
         <v>-1</v>
       </c>
       <c r="H25" s="1">
-        <v>-1</v>
-      </c>
-      <c r="I25" s="9">
+        <v>23</v>
+      </c>
+      <c r="I25" s="2">
         <v>-1</v>
       </c>
     </row>
@@ -1382,9 +1378,9 @@
         <v>-1</v>
       </c>
       <c r="H26" s="1">
-        <v>-1</v>
-      </c>
-      <c r="I26" s="9">
+        <v>24</v>
+      </c>
+      <c r="I26" s="2">
         <v>-1</v>
       </c>
     </row>
@@ -1411,10 +1407,10 @@
       <c r="G27" s="1">
         <v>-1</v>
       </c>
-      <c r="H27" s="1">
-        <v>-1</v>
-      </c>
-      <c r="I27" s="9">
+      <c r="H27" s="6">
+        <v>25</v>
+      </c>
+      <c r="I27" s="2">
         <v>-1</v>
       </c>
     </row>
@@ -1442,9 +1438,9 @@
         <v>-1</v>
       </c>
       <c r="H28" s="1">
-        <v>-1</v>
-      </c>
-      <c r="I28" s="9">
+        <v>26</v>
+      </c>
+      <c r="I28" s="2">
         <v>-1</v>
       </c>
     </row>
@@ -1471,10 +1467,10 @@
       <c r="G29" s="1">
         <v>-1</v>
       </c>
-      <c r="H29" s="1">
-        <v>-1</v>
-      </c>
-      <c r="I29" s="9">
+      <c r="H29" s="6">
+        <v>27</v>
+      </c>
+      <c r="I29" s="2">
         <v>-1</v>
       </c>
     </row>
@@ -1502,9 +1498,9 @@
         <v>-1</v>
       </c>
       <c r="H30" s="1">
-        <v>-1</v>
-      </c>
-      <c r="I30" s="9">
+        <v>28</v>
+      </c>
+      <c r="I30" s="2">
         <v>-1</v>
       </c>
     </row>
@@ -1532,9 +1528,9 @@
         <v>150</v>
       </c>
       <c r="H31" s="1">
-        <v>-1</v>
-      </c>
-      <c r="I31" s="9">
+        <v>29</v>
+      </c>
+      <c r="I31" s="2">
         <v>-1</v>
       </c>
     </row>
@@ -1561,10 +1557,10 @@
       <c r="G32" s="1">
         <v>-1</v>
       </c>
-      <c r="H32" s="1">
-        <v>-1</v>
-      </c>
-      <c r="I32" s="9">
+      <c r="H32" s="6">
+        <v>30</v>
+      </c>
+      <c r="I32" s="2">
         <v>-1</v>
       </c>
     </row>
@@ -1594,7 +1590,7 @@
       <c r="H33" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="I33" s="9">
+      <c r="I33" s="2">
         <v>-1</v>
       </c>
     </row>
@@ -1621,10 +1617,10 @@
       <c r="G34" s="1">
         <v>-1</v>
       </c>
-      <c r="H34" s="1">
-        <v>-1</v>
-      </c>
-      <c r="I34" s="9">
+      <c r="H34" s="6">
+        <v>32</v>
+      </c>
+      <c r="I34" s="2">
         <v>-1</v>
       </c>
     </row>
@@ -1652,9 +1648,9 @@
         <v>-1</v>
       </c>
       <c r="H35" s="1">
-        <v>-1</v>
-      </c>
-      <c r="I35" s="9">
+        <v>33</v>
+      </c>
+      <c r="I35" s="2">
         <v>-1</v>
       </c>
     </row>
@@ -1682,9 +1678,9 @@
         <v>-1</v>
       </c>
       <c r="H36" s="1">
-        <v>-1</v>
-      </c>
-      <c r="I36" s="9">
+        <v>34</v>
+      </c>
+      <c r="I36" s="2">
         <v>-1</v>
       </c>
     </row>
@@ -1711,10 +1707,10 @@
       <c r="G37" s="1">
         <v>-1</v>
       </c>
-      <c r="H37" s="1">
-        <v>-1</v>
-      </c>
-      <c r="I37" s="9">
+      <c r="H37" s="6">
+        <v>35</v>
+      </c>
+      <c r="I37" s="2">
         <v>-1</v>
       </c>
     </row>
@@ -1742,9 +1738,9 @@
         <v>-1</v>
       </c>
       <c r="H38" s="1">
-        <v>-1</v>
-      </c>
-      <c r="I38" s="9">
+        <v>36</v>
+      </c>
+      <c r="I38" s="2">
         <v>-1</v>
       </c>
     </row>
@@ -1772,9 +1768,9 @@
         <v>-1</v>
       </c>
       <c r="H39" s="1">
-        <v>-1</v>
-      </c>
-      <c r="I39" s="9">
+        <v>37</v>
+      </c>
+      <c r="I39" s="2">
         <v>-1</v>
       </c>
     </row>
@@ -1801,10 +1797,10 @@
       <c r="G40" s="1">
         <v>-1</v>
       </c>
-      <c r="H40" s="1">
-        <v>-1</v>
-      </c>
-      <c r="I40" s="9">
+      <c r="H40" s="6">
+        <v>38</v>
+      </c>
+      <c r="I40" s="2">
         <v>-1</v>
       </c>
     </row>
@@ -1834,7 +1830,7 @@
       <c r="H41" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="I41" s="9">
+      <c r="I41" s="2">
         <v>-1</v>
       </c>
     </row>
@@ -1862,9 +1858,9 @@
         <v>-1</v>
       </c>
       <c r="H42" s="1">
-        <v>-1</v>
-      </c>
-      <c r="I42" s="9">
+        <v>40</v>
+      </c>
+      <c r="I42" s="2">
         <v>-1</v>
       </c>
     </row>
@@ -1891,10 +1887,10 @@
       <c r="G43" s="1">
         <v>-1</v>
       </c>
-      <c r="H43" s="1">
-        <v>-1</v>
-      </c>
-      <c r="I43" s="9">
+      <c r="H43" s="6">
+        <v>41</v>
+      </c>
+      <c r="I43" s="2">
         <v>-1</v>
       </c>
     </row>
@@ -1922,9 +1918,9 @@
         <v>-1</v>
       </c>
       <c r="H44" s="1">
-        <v>-1</v>
-      </c>
-      <c r="I44" s="9">
+        <v>42</v>
+      </c>
+      <c r="I44" s="2">
         <v>-1</v>
       </c>
     </row>
@@ -1952,9 +1948,9 @@
         <v>-1</v>
       </c>
       <c r="H45" s="1">
-        <v>-1</v>
-      </c>
-      <c r="I45" s="9">
+        <v>43</v>
+      </c>
+      <c r="I45" s="2">
         <v>-1</v>
       </c>
     </row>
@@ -1981,10 +1977,10 @@
       <c r="G46" s="1">
         <v>-1</v>
       </c>
-      <c r="H46" s="1">
-        <v>-1</v>
-      </c>
-      <c r="I46" s="9">
+      <c r="H46" s="6">
+        <v>44</v>
+      </c>
+      <c r="I46" s="2">
         <v>-1</v>
       </c>
     </row>
@@ -2012,9 +2008,9 @@
         <v>-1</v>
       </c>
       <c r="H47" s="1">
-        <v>-1</v>
-      </c>
-      <c r="I47" s="9">
+        <v>45</v>
+      </c>
+      <c r="I47" s="2">
         <v>-1</v>
       </c>
     </row>
@@ -2042,9 +2038,9 @@
         <v>-1</v>
       </c>
       <c r="H48" s="1">
-        <v>-1</v>
-      </c>
-      <c r="I48" s="9">
+        <v>46</v>
+      </c>
+      <c r="I48" s="2">
         <v>-1</v>
       </c>
     </row>
@@ -2071,10 +2067,10 @@
       <c r="G49" s="1">
         <v>-1</v>
       </c>
-      <c r="H49" s="1">
-        <v>-1</v>
-      </c>
-      <c r="I49" s="9">
+      <c r="H49" s="6">
+        <v>47</v>
+      </c>
+      <c r="I49" s="2">
         <v>-1</v>
       </c>
     </row>
@@ -2104,7 +2100,7 @@
       <c r="H50" s="7" t="s">
         <v>26</v>
       </c>
-      <c r="I50" s="9">
+      <c r="I50" s="2">
         <v>-1</v>
       </c>
     </row>
@@ -2132,9 +2128,9 @@
         <v>-1</v>
       </c>
       <c r="H51" s="1">
-        <v>-1</v>
-      </c>
-      <c r="I51" s="9">
+        <v>49</v>
+      </c>
+      <c r="I51" s="2">
         <v>-1</v>
       </c>
     </row>
@@ -2161,10 +2157,10 @@
       <c r="G52" s="1">
         <v>-1</v>
       </c>
-      <c r="H52" s="1">
-        <v>-1</v>
-      </c>
-      <c r="I52" s="9">
+      <c r="H52" s="6">
+        <v>50</v>
+      </c>
+      <c r="I52" s="2">
         <v>-1</v>
       </c>
     </row>
@@ -2192,9 +2188,9 @@
         <v>-1</v>
       </c>
       <c r="H53" s="1">
-        <v>-1</v>
-      </c>
-      <c r="I53" s="9">
+        <v>51</v>
+      </c>
+      <c r="I53" s="2">
         <v>-1</v>
       </c>
     </row>
@@ -2222,9 +2218,9 @@
         <v>-1</v>
       </c>
       <c r="H54" s="1">
-        <v>-1</v>
-      </c>
-      <c r="I54" s="9">
+        <v>52</v>
+      </c>
+      <c r="I54" s="2">
         <v>-1</v>
       </c>
     </row>
@@ -2251,10 +2247,10 @@
       <c r="G55" s="1">
         <v>-1</v>
       </c>
-      <c r="H55" s="1">
-        <v>-1</v>
-      </c>
-      <c r="I55" s="9">
+      <c r="H55" s="6">
+        <v>53</v>
+      </c>
+      <c r="I55" s="2">
         <v>-1</v>
       </c>
     </row>
@@ -2282,9 +2278,9 @@
         <v>-1</v>
       </c>
       <c r="H56" s="1">
-        <v>-1</v>
-      </c>
-      <c r="I56" s="9">
+        <v>54</v>
+      </c>
+      <c r="I56" s="2">
         <v>-1</v>
       </c>
     </row>
@@ -2312,9 +2308,9 @@
         <v>-1</v>
       </c>
       <c r="H57" s="1">
-        <v>-1</v>
-      </c>
-      <c r="I57" s="9">
+        <v>55</v>
+      </c>
+      <c r="I57" s="2">
         <v>-1</v>
       </c>
     </row>
@@ -2341,10 +2337,10 @@
       <c r="G58" s="1">
         <v>-1</v>
       </c>
-      <c r="H58" s="1">
-        <v>-1</v>
-      </c>
-      <c r="I58" s="9">
+      <c r="H58" s="6">
+        <v>56</v>
+      </c>
+      <c r="I58" s="2">
         <v>-1</v>
       </c>
     </row>
@@ -2374,7 +2370,7 @@
       <c r="H59" s="7" t="s">
         <v>27</v>
       </c>
-      <c r="I59" s="9">
+      <c r="I59" s="2">
         <v>-1</v>
       </c>
     </row>
@@ -2402,9 +2398,9 @@
         <v>-1</v>
       </c>
       <c r="H60" s="1">
-        <v>-1</v>
-      </c>
-      <c r="I60" s="9">
+        <v>58</v>
+      </c>
+      <c r="I60" s="2">
         <v>-1</v>
       </c>
     </row>
@@ -2431,10 +2427,10 @@
       <c r="G61" s="1">
         <v>-1</v>
       </c>
-      <c r="H61" s="1">
-        <v>-1</v>
-      </c>
-      <c r="I61" s="9">
+      <c r="H61" s="6">
+        <v>59</v>
+      </c>
+      <c r="I61" s="2">
         <v>-1</v>
       </c>
     </row>
@@ -2462,9 +2458,9 @@
         <v>-1</v>
       </c>
       <c r="H62" s="1">
-        <v>-1</v>
-      </c>
-      <c r="I62" s="9">
+        <v>60</v>
+      </c>
+      <c r="I62" s="2">
         <v>-1</v>
       </c>
     </row>
@@ -2492,9 +2488,9 @@
         <v>-1</v>
       </c>
       <c r="H63" s="1">
-        <v>-1</v>
-      </c>
-      <c r="I63" s="9">
+        <v>61</v>
+      </c>
+      <c r="I63" s="2">
         <v>-1</v>
       </c>
     </row>
@@ -2521,10 +2517,10 @@
       <c r="G64" s="1">
         <v>-1</v>
       </c>
-      <c r="H64" s="7">
-        <v>-1</v>
-      </c>
-      <c r="I64" s="9">
+      <c r="H64" s="6">
+        <v>62</v>
+      </c>
+      <c r="I64" s="2">
         <v>-1</v>
       </c>
     </row>
@@ -2552,9 +2548,9 @@
         <v>62</v>
       </c>
       <c r="H65" s="1">
-        <v>-1</v>
-      </c>
-      <c r="I65" s="9">
+        <v>63</v>
+      </c>
+      <c r="I65" s="2">
         <v>-1</v>
       </c>
     </row>
@@ -2582,9 +2578,9 @@
         <v>-1</v>
       </c>
       <c r="H66" s="1">
-        <v>-1</v>
-      </c>
-      <c r="I66" s="9">
+        <v>64</v>
+      </c>
+      <c r="I66" s="2">
         <v>-1</v>
       </c>
     </row>
@@ -2614,7 +2610,7 @@
       <c r="H67" s="7" t="s">
         <v>30</v>
       </c>
-      <c r="I67" s="9">
+      <c r="I67" s="2">
         <v>-1</v>
       </c>
     </row>
@@ -2642,9 +2638,9 @@
         <v>-1</v>
       </c>
       <c r="H68" s="1">
-        <v>-1</v>
-      </c>
-      <c r="I68" s="9">
+        <v>66</v>
+      </c>
+      <c r="I68" s="2">
         <v>-1</v>
       </c>
     </row>
@@ -2672,9 +2668,9 @@
         <v>-1</v>
       </c>
       <c r="H69" s="1">
-        <v>-1</v>
-      </c>
-      <c r="I69" s="9">
+        <v>67</v>
+      </c>
+      <c r="I69" s="2">
         <v>-1</v>
       </c>
     </row>
@@ -2701,10 +2697,10 @@
       <c r="G70" s="1">
         <v>-1</v>
       </c>
-      <c r="H70" s="1">
-        <v>-1</v>
-      </c>
-      <c r="I70" s="9">
+      <c r="H70" s="6">
+        <v>68</v>
+      </c>
+      <c r="I70" s="2">
         <v>-1</v>
       </c>
     </row>
@@ -2732,9 +2728,9 @@
         <v>-1</v>
       </c>
       <c r="H71" s="1">
-        <v>-1</v>
-      </c>
-      <c r="I71" s="9">
+        <v>69</v>
+      </c>
+      <c r="I71" s="2">
         <v>-1</v>
       </c>
     </row>
@@ -2761,10 +2757,10 @@
       <c r="G72" s="1">
         <v>-1</v>
       </c>
-      <c r="H72" s="7">
-        <v>-1</v>
-      </c>
-      <c r="I72" s="9">
+      <c r="H72" s="1">
+        <v>70</v>
+      </c>
+      <c r="I72" s="2">
         <v>-1</v>
       </c>
     </row>
@@ -2791,10 +2787,10 @@
       <c r="G73" s="1">
         <v>-1</v>
       </c>
-      <c r="H73" s="1">
-        <v>-1</v>
-      </c>
-      <c r="I73" s="9">
+      <c r="H73" s="6">
+        <v>71</v>
+      </c>
+      <c r="I73" s="2">
         <v>-1</v>
       </c>
     </row>
@@ -2822,9 +2818,9 @@
         <v>-1</v>
       </c>
       <c r="H74" s="1">
-        <v>-1</v>
-      </c>
-      <c r="I74" s="9">
+        <v>72</v>
+      </c>
+      <c r="I74" s="2">
         <v>-1</v>
       </c>
     </row>
@@ -2854,7 +2850,7 @@
       <c r="H75" s="7" t="s">
         <v>32</v>
       </c>
-      <c r="I75" s="9">
+      <c r="I75" s="2">
         <v>-1</v>
       </c>
     </row>
@@ -2881,10 +2877,10 @@
       <c r="G76" s="1">
         <v>-1</v>
       </c>
-      <c r="H76" s="1">
-        <v>-1</v>
-      </c>
-      <c r="I76" s="9">
+      <c r="H76" s="6">
+        <v>74</v>
+      </c>
+      <c r="I76" s="2">
         <v>-1</v>
       </c>
     </row>
@@ -2912,9 +2908,9 @@
         <v>-1</v>
       </c>
       <c r="H77" s="1">
-        <v>-1</v>
-      </c>
-      <c r="I77" s="9">
+        <v>75</v>
+      </c>
+      <c r="I77" s="2">
         <v>-1</v>
       </c>
     </row>
@@ -2942,9 +2938,9 @@
         <v>-1</v>
       </c>
       <c r="H78" s="1">
-        <v>-1</v>
-      </c>
-      <c r="I78" s="9">
+        <v>76</v>
+      </c>
+      <c r="I78" s="2">
         <v>-1</v>
       </c>
     </row>
@@ -2974,7 +2970,7 @@
       <c r="H79" s="7" t="s">
         <v>35</v>
       </c>
-      <c r="I79" s="9">
+      <c r="I79" s="2">
         <v>-1</v>
       </c>
     </row>
@@ -3001,10 +2997,10 @@
       <c r="G80" s="1">
         <v>-1</v>
       </c>
-      <c r="H80" s="1">
-        <v>-1</v>
-      </c>
-      <c r="I80" s="9">
+      <c r="H80" s="6">
+        <v>78</v>
+      </c>
+      <c r="I80" s="2">
         <v>-1</v>
       </c>
     </row>
@@ -3032,9 +3028,9 @@
         <v>-1</v>
       </c>
       <c r="H81" s="1">
-        <v>-1</v>
-      </c>
-      <c r="I81" s="9">
+        <v>79</v>
+      </c>
+      <c r="I81" s="2">
         <v>-1</v>
       </c>
     </row>
@@ -3062,9 +3058,9 @@
         <v>-1</v>
       </c>
       <c r="H82" s="1">
-        <v>-1</v>
-      </c>
-      <c r="I82" s="9">
+        <v>80</v>
+      </c>
+      <c r="I82" s="2">
         <v>-1</v>
       </c>
     </row>
@@ -3091,10 +3087,10 @@
       <c r="G83" s="1">
         <v>-1</v>
       </c>
-      <c r="H83" s="7">
-        <v>-1</v>
-      </c>
-      <c r="I83" s="9">
+      <c r="H83" s="1">
+        <v>81</v>
+      </c>
+      <c r="I83" s="2">
         <v>-1</v>
       </c>
     </row>
@@ -3121,10 +3117,10 @@
       <c r="G84" s="1">
         <v>-1</v>
       </c>
-      <c r="H84" s="1">
-        <v>-1</v>
-      </c>
-      <c r="I84" s="9">
+      <c r="H84" s="6">
+        <v>82</v>
+      </c>
+      <c r="I84" s="2">
         <v>-1</v>
       </c>
     </row>
@@ -3152,9 +3148,9 @@
         <v>-1</v>
       </c>
       <c r="H85" s="1">
-        <v>-1</v>
-      </c>
-      <c r="I85" s="9">
+        <v>83</v>
+      </c>
+      <c r="I85" s="2">
         <v>-1</v>
       </c>
     </row>
@@ -3182,9 +3178,9 @@
         <v>-1</v>
       </c>
       <c r="H86" s="1">
-        <v>-1</v>
-      </c>
-      <c r="I86" s="9">
+        <v>84</v>
+      </c>
+      <c r="I86" s="2">
         <v>-1</v>
       </c>
     </row>
@@ -3212,9 +3208,9 @@
         <v>100</v>
       </c>
       <c r="H87" s="1">
-        <v>-1</v>
-      </c>
-      <c r="I87" s="9">
+        <v>85</v>
+      </c>
+      <c r="I87" s="2">
         <v>-1</v>
       </c>
     </row>
@@ -3241,10 +3237,10 @@
       <c r="G88" s="1">
         <v>-1</v>
       </c>
-      <c r="H88" s="1">
-        <v>-1</v>
-      </c>
-      <c r="I88" s="9">
+      <c r="H88" s="6">
+        <v>86</v>
+      </c>
+      <c r="I88" s="2">
         <v>-1</v>
       </c>
     </row>
@@ -3272,9 +3268,9 @@
         <v>-1</v>
       </c>
       <c r="H89" s="1">
-        <v>-1</v>
-      </c>
-      <c r="I89" s="9">
+        <v>87</v>
+      </c>
+      <c r="I89" s="2">
         <v>-1</v>
       </c>
     </row>
@@ -3304,7 +3300,7 @@
       <c r="H90" s="7" t="s">
         <v>37</v>
       </c>
-      <c r="I90" s="9">
+      <c r="I90" s="2">
         <v>-1</v>
       </c>
     </row>
@@ -3331,10 +3327,10 @@
       <c r="G91" s="1">
         <v>-1</v>
       </c>
-      <c r="H91" s="7">
-        <v>-1</v>
-      </c>
-      <c r="I91" s="9">
+      <c r="H91" s="1">
+        <v>89</v>
+      </c>
+      <c r="I91" s="2">
         <v>-1</v>
       </c>
     </row>
@@ -3361,10 +3357,10 @@
       <c r="G92" s="1">
         <v>-1</v>
       </c>
-      <c r="H92" s="1">
-        <v>-1</v>
-      </c>
-      <c r="I92" s="9">
+      <c r="H92" s="6">
+        <v>90</v>
+      </c>
+      <c r="I92" s="2">
         <v>-1</v>
       </c>
     </row>
@@ -3392,9 +3388,9 @@
         <v>-1</v>
       </c>
       <c r="H93" s="1">
-        <v>-1</v>
-      </c>
-      <c r="I93" s="9">
+        <v>91</v>
+      </c>
+      <c r="I93" s="2">
         <v>-1</v>
       </c>
     </row>
@@ -3422,9 +3418,9 @@
         <v>-1</v>
       </c>
       <c r="H94" s="1">
-        <v>-1</v>
-      </c>
-      <c r="I94" s="9">
+        <v>92</v>
+      </c>
+      <c r="I94" s="2">
         <v>-1</v>
       </c>
     </row>
@@ -3452,9 +3448,9 @@
         <v>-1</v>
       </c>
       <c r="H95" s="1">
-        <v>-1</v>
-      </c>
-      <c r="I95" s="9">
+        <v>93</v>
+      </c>
+      <c r="I95" s="2">
         <v>-1</v>
       </c>
     </row>
@@ -3481,10 +3477,10 @@
       <c r="G96" s="1">
         <v>-1</v>
       </c>
-      <c r="H96" s="1">
-        <v>-1</v>
-      </c>
-      <c r="I96" s="9">
+      <c r="H96" s="6">
+        <v>94</v>
+      </c>
+      <c r="I96" s="2">
         <v>-1</v>
       </c>
     </row>
@@ -3512,9 +3508,9 @@
         <v>-1</v>
       </c>
       <c r="H97" s="1">
-        <v>-1</v>
-      </c>
-      <c r="I97" s="9">
+        <v>95</v>
+      </c>
+      <c r="I97" s="2">
         <v>-1</v>
       </c>
     </row>
@@ -3544,7 +3540,7 @@
       <c r="H98" s="7" t="s">
         <v>39</v>
       </c>
-      <c r="I98" s="9">
+      <c r="I98" s="2">
         <v>-1</v>
       </c>
     </row>
@@ -3571,10 +3567,10 @@
       <c r="G99" s="1">
         <v>-1</v>
       </c>
-      <c r="H99" s="7">
-        <v>-1</v>
-      </c>
-      <c r="I99" s="9">
+      <c r="H99" s="1">
+        <v>97</v>
+      </c>
+      <c r="I99" s="2">
         <v>-1</v>
       </c>
     </row>
@@ -3601,10 +3597,10 @@
       <c r="G100" s="1">
         <v>-1</v>
       </c>
-      <c r="H100" s="1">
-        <v>-1</v>
-      </c>
-      <c r="I100" s="9">
+      <c r="H100" s="6">
+        <v>98</v>
+      </c>
+      <c r="I100" s="2">
         <v>-1</v>
       </c>
     </row>
@@ -3632,9 +3628,9 @@
         <v>-1</v>
       </c>
       <c r="H101" s="1">
-        <v>-1</v>
-      </c>
-      <c r="I101" s="9">
+        <v>99</v>
+      </c>
+      <c r="I101" s="2">
         <v>-1</v>
       </c>
     </row>
@@ -3662,9 +3658,9 @@
         <v>-1</v>
       </c>
       <c r="H102" s="1">
-        <v>-1</v>
-      </c>
-      <c r="I102" s="9">
+        <v>100</v>
+      </c>
+      <c r="I102" s="2">
         <v>-1</v>
       </c>
     </row>
@@ -3692,9 +3688,9 @@
         <v>-1</v>
       </c>
       <c r="H103" s="1">
-        <v>-1</v>
-      </c>
-      <c r="I103" s="9">
+        <v>101</v>
+      </c>
+      <c r="I103" s="2">
         <v>-1</v>
       </c>
     </row>
@@ -3721,10 +3717,10 @@
       <c r="G104" s="1">
         <v>-1</v>
       </c>
-      <c r="H104" s="1">
-        <v>-1</v>
-      </c>
-      <c r="I104" s="9">
+      <c r="H104" s="6">
+        <v>102</v>
+      </c>
+      <c r="I104" s="2">
         <v>-1</v>
       </c>
     </row>
@@ -3752,9 +3748,9 @@
         <v>-1</v>
       </c>
       <c r="H105" s="1">
-        <v>-1</v>
-      </c>
-      <c r="I105" s="9">
+        <v>103</v>
+      </c>
+      <c r="I105" s="2">
         <v>-1</v>
       </c>
     </row>
@@ -3782,9 +3778,9 @@
         <v>-1</v>
       </c>
       <c r="H106" s="1">
-        <v>-1</v>
-      </c>
-      <c r="I106" s="9">
+        <v>104</v>
+      </c>
+      <c r="I106" s="2">
         <v>-1</v>
       </c>
     </row>
@@ -3814,7 +3810,7 @@
       <c r="H107" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="I107" s="9">
+      <c r="I107" s="2">
         <v>-1</v>
       </c>
     </row>
@@ -3841,10 +3837,10 @@
       <c r="G108" s="1">
         <v>-1</v>
       </c>
-      <c r="H108" s="7">
-        <v>-1</v>
-      </c>
-      <c r="I108" s="9">
+      <c r="H108" s="6">
+        <v>106</v>
+      </c>
+      <c r="I108" s="2">
         <v>-1</v>
       </c>
     </row>
@@ -3872,9 +3868,9 @@
         <v>-1</v>
       </c>
       <c r="H109" s="1">
-        <v>-1</v>
-      </c>
-      <c r="I109" s="9">
+        <v>107</v>
+      </c>
+      <c r="I109" s="2">
         <v>-1</v>
       </c>
     </row>
@@ -3902,9 +3898,9 @@
         <v>-1</v>
       </c>
       <c r="H110" s="1">
-        <v>-1</v>
-      </c>
-      <c r="I110" s="9">
+        <v>108</v>
+      </c>
+      <c r="I110" s="2">
         <v>-1</v>
       </c>
     </row>
@@ -3932,9 +3928,9 @@
         <v>-1</v>
       </c>
       <c r="H111" s="1">
-        <v>-1</v>
-      </c>
-      <c r="I111" s="9">
+        <v>109</v>
+      </c>
+      <c r="I111" s="2">
         <v>-1</v>
       </c>
     </row>
@@ -3961,10 +3957,10 @@
       <c r="G112" s="1">
         <v>-1</v>
       </c>
-      <c r="H112" s="1">
-        <v>-1</v>
-      </c>
-      <c r="I112" s="9">
+      <c r="H112" s="6">
+        <v>110</v>
+      </c>
+      <c r="I112" s="2">
         <v>-1</v>
       </c>
     </row>
@@ -3992,9 +3988,9 @@
         <v>-1</v>
       </c>
       <c r="H113" s="1">
-        <v>-1</v>
-      </c>
-      <c r="I113" s="9">
+        <v>111</v>
+      </c>
+      <c r="I113" s="2">
         <v>-1</v>
       </c>
     </row>
@@ -4022,9 +4018,9 @@
         <v>-1</v>
       </c>
       <c r="H114" s="1">
-        <v>-1</v>
-      </c>
-      <c r="I114" s="9">
+        <v>112</v>
+      </c>
+      <c r="I114" s="2">
         <v>-1</v>
       </c>
     </row>
@@ -4052,9 +4048,9 @@
         <v>-1</v>
       </c>
       <c r="H115" s="1">
-        <v>-1</v>
-      </c>
-      <c r="I115" s="9">
+        <v>113</v>
+      </c>
+      <c r="I115" s="2">
         <v>-1</v>
       </c>
     </row>
@@ -4085,7 +4081,7 @@
       <c r="H116" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="I116" s="9">
+      <c r="I116" s="2">
         <v>-1</v>
       </c>
     </row>
@@ -4112,10 +4108,10 @@
       <c r="G117" s="1">
         <v>-1</v>
       </c>
-      <c r="H117" s="7">
-        <v>-1</v>
-      </c>
-      <c r="I117" s="9">
+      <c r="H117" s="1">
+        <v>115</v>
+      </c>
+      <c r="I117" s="2">
         <v>-1</v>
       </c>
     </row>
@@ -4143,9 +4139,9 @@
         <v>-1</v>
       </c>
       <c r="H118" s="1">
-        <v>-1</v>
-      </c>
-      <c r="I118" s="9">
+        <v>116</v>
+      </c>
+      <c r="I118" s="2">
         <v>-1</v>
       </c>
     </row>
@@ -4173,9 +4169,9 @@
         <v>-1</v>
       </c>
       <c r="H119" s="1">
-        <v>-1</v>
-      </c>
-      <c r="I119" s="9">
+        <v>117</v>
+      </c>
+      <c r="I119" s="2">
         <v>-1</v>
       </c>
     </row>
@@ -4202,10 +4198,10 @@
       <c r="G120" s="1">
         <v>-1</v>
       </c>
-      <c r="H120" s="1">
-        <v>-1</v>
-      </c>
-      <c r="I120" s="9">
+      <c r="H120" s="6">
+        <v>118</v>
+      </c>
+      <c r="I120" s="2">
         <v>-1</v>
       </c>
     </row>
@@ -4233,9 +4229,9 @@
         <v>-1</v>
       </c>
       <c r="H121" s="1">
-        <v>-1</v>
-      </c>
-      <c r="I121" s="9">
+        <v>119</v>
+      </c>
+      <c r="I121" s="2">
         <v>-1</v>
       </c>
     </row>
@@ -4263,9 +4259,9 @@
         <v>-1</v>
       </c>
       <c r="H122" s="1">
-        <v>-1</v>
-      </c>
-      <c r="I122" s="9">
+        <v>120</v>
+      </c>
+      <c r="I122" s="2">
         <v>-1</v>
       </c>
     </row>
@@ -4293,9 +4289,9 @@
         <v>-1</v>
       </c>
       <c r="H123" s="1">
-        <v>-1</v>
-      </c>
-      <c r="I123" s="9">
+        <v>121</v>
+      </c>
+      <c r="I123" s="2">
         <v>-1</v>
       </c>
     </row>
@@ -4322,10 +4318,10 @@
       <c r="G124" s="1">
         <v>-1</v>
       </c>
-      <c r="H124" s="1">
-        <v>-1</v>
-      </c>
-      <c r="I124" s="9">
+      <c r="H124" s="6">
+        <v>122</v>
+      </c>
+      <c r="I124" s="2">
         <v>-1</v>
       </c>
     </row>
@@ -4355,7 +4351,7 @@
       <c r="H125" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="I125" s="9">
+      <c r="I125" s="2">
         <v>-1</v>
       </c>
     </row>
@@ -4382,10 +4378,10 @@
       <c r="G126" s="1">
         <v>-1</v>
       </c>
-      <c r="H126" s="7">
-        <v>-1</v>
-      </c>
-      <c r="I126" s="9">
+      <c r="H126" s="1">
+        <v>124</v>
+      </c>
+      <c r="I126" s="2">
         <v>-1</v>
       </c>
     </row>
@@ -4413,9 +4409,9 @@
         <v>-1</v>
       </c>
       <c r="H127" s="1">
-        <v>-1</v>
-      </c>
-      <c r="I127" s="9">
+        <v>125</v>
+      </c>
+      <c r="I127" s="2">
         <v>-1</v>
       </c>
     </row>
@@ -4442,10 +4438,10 @@
       <c r="G128" s="1">
         <v>-1</v>
       </c>
-      <c r="H128" s="1">
-        <v>-1</v>
-      </c>
-      <c r="I128" s="9">
+      <c r="H128" s="6">
+        <v>126</v>
+      </c>
+      <c r="I128" s="2">
         <v>-1</v>
       </c>
     </row>
@@ -4473,9 +4469,9 @@
         <v>-1</v>
       </c>
       <c r="H129" s="1">
-        <v>-1</v>
-      </c>
-      <c r="I129" s="9">
+        <v>127</v>
+      </c>
+      <c r="I129" s="2">
         <v>-1</v>
       </c>
     </row>
@@ -4503,9 +4499,9 @@
         <v>-1</v>
       </c>
       <c r="H130" s="1">
-        <v>-1</v>
-      </c>
-      <c r="I130" s="9">
+        <v>128</v>
+      </c>
+      <c r="I130" s="2">
         <v>-1</v>
       </c>
     </row>
@@ -4533,9 +4529,9 @@
         <v>-1</v>
       </c>
       <c r="H131" s="1">
-        <v>-1</v>
-      </c>
-      <c r="I131" s="9">
+        <v>129</v>
+      </c>
+      <c r="I131" s="2">
         <v>-1</v>
       </c>
     </row>
@@ -4562,10 +4558,10 @@
       <c r="G132" s="1">
         <v>-1</v>
       </c>
-      <c r="H132" s="1">
-        <v>-1</v>
-      </c>
-      <c r="I132" s="9">
+      <c r="H132" s="6">
+        <v>130</v>
+      </c>
+      <c r="I132" s="2">
         <v>-1</v>
       </c>
     </row>
@@ -4593,9 +4589,9 @@
         <v>-1</v>
       </c>
       <c r="H133" s="1">
-        <v>-1</v>
-      </c>
-      <c r="I133" s="9">
+        <v>131</v>
+      </c>
+      <c r="I133" s="2">
         <v>-1</v>
       </c>
     </row>
@@ -4625,7 +4621,7 @@
       <c r="H134" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="I134" s="9">
+      <c r="I134" s="2">
         <v>-1</v>
       </c>
     </row>
@@ -4652,10 +4648,10 @@
       <c r="G135" s="1">
         <v>-1</v>
       </c>
-      <c r="H135" s="7">
-        <v>-1</v>
-      </c>
-      <c r="I135" s="9">
+      <c r="H135" s="1">
+        <v>133</v>
+      </c>
+      <c r="I135" s="2">
         <v>-1</v>
       </c>
     </row>
@@ -4682,10 +4678,10 @@
       <c r="G136" s="1">
         <v>-1</v>
       </c>
-      <c r="H136" s="1">
-        <v>-1</v>
-      </c>
-      <c r="I136" s="9">
+      <c r="H136" s="6">
+        <v>134</v>
+      </c>
+      <c r="I136" s="2">
         <v>-1</v>
       </c>
     </row>
@@ -4713,9 +4709,9 @@
         <v>-1</v>
       </c>
       <c r="H137" s="1">
-        <v>-1</v>
-      </c>
-      <c r="I137" s="9">
+        <v>135</v>
+      </c>
+      <c r="I137" s="2">
         <v>-1</v>
       </c>
     </row>
@@ -4743,9 +4739,9 @@
         <v>-1</v>
       </c>
       <c r="H138" s="1">
-        <v>-1</v>
-      </c>
-      <c r="I138" s="9">
+        <v>136</v>
+      </c>
+      <c r="I138" s="2">
         <v>-1</v>
       </c>
     </row>
@@ -4773,9 +4769,9 @@
         <v>-1</v>
       </c>
       <c r="H139" s="1">
-        <v>-1</v>
-      </c>
-      <c r="I139" s="9">
+        <v>137</v>
+      </c>
+      <c r="I139" s="2">
         <v>-1</v>
       </c>
     </row>
@@ -4802,10 +4798,10 @@
       <c r="G140" s="1">
         <v>-1</v>
       </c>
-      <c r="H140" s="1">
-        <v>-1</v>
-      </c>
-      <c r="I140" s="9">
+      <c r="H140" s="6">
+        <v>138</v>
+      </c>
+      <c r="I140" s="2">
         <v>-1</v>
       </c>
     </row>
@@ -4833,9 +4829,9 @@
         <v>-1</v>
       </c>
       <c r="H141" s="1">
-        <v>-1</v>
-      </c>
-      <c r="I141" s="9">
+        <v>139</v>
+      </c>
+      <c r="I141" s="2">
         <v>-1</v>
       </c>
     </row>
@@ -4863,9 +4859,9 @@
         <v>-1</v>
       </c>
       <c r="H142" s="1">
-        <v>-1</v>
-      </c>
-      <c r="I142" s="9">
+        <v>140</v>
+      </c>
+      <c r="I142" s="2">
         <v>-1</v>
       </c>
     </row>
@@ -4895,7 +4891,7 @@
       <c r="H143" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="I143" s="9">
+      <c r="I143" s="2">
         <v>-1</v>
       </c>
     </row>
@@ -4922,10 +4918,10 @@
       <c r="G144" s="1">
         <v>-1</v>
       </c>
-      <c r="H144" s="7">
-        <v>-1</v>
-      </c>
-      <c r="I144" s="9">
+      <c r="H144" s="6">
+        <v>142</v>
+      </c>
+      <c r="I144" s="2">
         <v>-1</v>
       </c>
     </row>
@@ -4953,9 +4949,9 @@
         <v>-1</v>
       </c>
       <c r="H145" s="1">
-        <v>-1</v>
-      </c>
-      <c r="I145" s="9">
+        <v>143</v>
+      </c>
+      <c r="I145" s="2">
         <v>-1</v>
       </c>
     </row>
@@ -4983,9 +4979,9 @@
         <v>-1</v>
       </c>
       <c r="H146" s="1">
-        <v>-1</v>
-      </c>
-      <c r="I146" s="9">
+        <v>144</v>
+      </c>
+      <c r="I146" s="2">
         <v>-1</v>
       </c>
     </row>
@@ -5013,9 +5009,9 @@
         <v>-1</v>
       </c>
       <c r="H147" s="1">
-        <v>-1</v>
-      </c>
-      <c r="I147" s="9">
+        <v>145</v>
+      </c>
+      <c r="I147" s="2">
         <v>-1</v>
       </c>
     </row>
@@ -5042,10 +5038,10 @@
       <c r="G148" s="1">
         <v>-1</v>
       </c>
-      <c r="H148" s="1">
-        <v>-1</v>
-      </c>
-      <c r="I148" s="9">
+      <c r="H148" s="6">
+        <v>146</v>
+      </c>
+      <c r="I148" s="2">
         <v>-1</v>
       </c>
     </row>
@@ -5073,9 +5069,9 @@
         <v>-1</v>
       </c>
       <c r="H149" s="1">
-        <v>-1</v>
-      </c>
-      <c r="I149" s="9">
+        <v>147</v>
+      </c>
+      <c r="I149" s="2">
         <v>-1</v>
       </c>
     </row>
@@ -5104,9 +5100,9 @@
         <v>-1</v>
       </c>
       <c r="H150" s="1">
-        <v>-1</v>
-      </c>
-      <c r="I150" s="9">
+        <v>148</v>
+      </c>
+      <c r="I150" s="2">
         <v>-1</v>
       </c>
     </row>
@@ -5134,9 +5130,9 @@
         <v>-1</v>
       </c>
       <c r="H151" s="1">
-        <v>-1</v>
-      </c>
-      <c r="I151" s="9">
+        <v>149</v>
+      </c>
+      <c r="I151" s="2">
         <v>-1</v>
       </c>
     </row>
@@ -5163,10 +5159,10 @@
       <c r="G152" s="1">
         <v>-1</v>
       </c>
-      <c r="H152" s="1">
-        <v>-1</v>
-      </c>
-      <c r="I152" s="9">
+      <c r="H152" s="6">
+        <v>150</v>
+      </c>
+      <c r="I152" s="2">
         <v>-1</v>
       </c>
     </row>

</xml_diff>